<commit_message>
Agrego diagrama de arquitecura y algunos cambios en los demas diagramas
</commit_message>
<xml_diff>
--- a/Documentacion/Tabla de requerimientos no funcionales.xlsx
+++ b/Documentacion/Tabla de requerimientos no funcionales.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500800_{D15830F6-4CAC-4296-BFD9-2AA7D424B7E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Codigo</t>
   </si>
@@ -146,13 +148,22 @@
   </si>
   <si>
     <t>Tolerancia a fallos</t>
+  </si>
+  <si>
+    <t>Cantidad de usuarios</t>
+  </si>
+  <si>
+    <t>Contemplar que el sistema soporte la cantidad de usuarios necesarios sin afectar el desempeño de la aplcacion</t>
+  </si>
+  <si>
+    <t>Escalabilidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,11 +245,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -280,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -312,9 +331,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,6 +383,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,21 +576,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -549,7 +604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -563,7 +618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -578,7 +633,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="30">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -593,7 +648,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -608,7 +663,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="75">
+    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -623,7 +678,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="45">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,7 +697,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="60">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -661,20 +716,26 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -682,7 +743,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -690,7 +751,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -698,7 +759,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -706,7 +767,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -714,7 +775,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -722,7 +783,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -730,7 +791,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -738,7 +799,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -746,7 +807,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -754,7 +815,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -762,7 +823,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -778,12 +839,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -791,12 +852,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>